<commit_message>
Password and retype password field test cases updated
</commit_message>
<xml_diff>
--- a/Test Case for Bdjobs Create Account.xlsx
+++ b/Test Case for Bdjobs Create Account.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="140">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -185,31 +185,59 @@
     <t>TC_14</t>
   </si>
   <si>
+    <t>!@#$%</t>
+  </si>
+  <si>
     <t>TC_15</t>
   </si>
   <si>
+    <t>123$%&amp;*</t>
+  </si>
+  <si>
     <t>TC_16</t>
   </si>
   <si>
+    <t>123asdf</t>
+  </si>
+  <si>
     <t>TC_17</t>
   </si>
   <si>
+    <t>123~!@#</t>
+  </si>
+  <si>
     <t>TC_18</t>
   </si>
   <si>
+    <t>ABC</t>
+  </si>
+  <si>
     <t>TC_19</t>
   </si>
   <si>
+    <t>abc</t>
+  </si>
+  <si>
     <t>TC_20</t>
   </si>
   <si>
     <t>Check the lenght limitations</t>
   </si>
   <si>
+    <t>asdfghjklQWERTYUIOPZXCVBNM@gmail.com</t>
+  </si>
+  <si>
     <t>TC_21</t>
   </si>
   <si>
     <t>TC_22</t>
+  </si>
+  <si>
+    <t>Check the field is case-sensitive or not for valid 
+mail</t>
+  </si>
+  <si>
+    <t>fUaDDapurBo00@gmail.com</t>
   </si>
   <si>
     <t>TC_23</t>
@@ -219,6 +247,9 @@
 @ or not</t>
   </si>
   <si>
+    <t>fuaddapurbo00gmail.com</t>
+  </si>
+  <si>
     <t>TC_24</t>
   </si>
   <si>
@@ -226,6 +257,9 @@
 name or not</t>
   </si>
   <si>
+    <t>fuaddapurbo00@.com</t>
+  </si>
+  <si>
     <t>TC_25</t>
   </si>
   <si>
@@ -233,6 +267,9 @@
 name or not</t>
   </si>
   <si>
+    <t>@gmail.com</t>
+  </si>
+  <si>
     <t>TC_26</t>
   </si>
   <si>
@@ -240,18 +277,193 @@
 not</t>
   </si>
   <si>
+    <t>fuaddapurbo00@asdfgssd12345.com</t>
+  </si>
+  <si>
     <t>TC_27</t>
   </si>
   <si>
     <t>Check the field accepts extra @ in the address or 
 not</t>
+  </si>
+  <si>
+    <t>fuaddapurbo00@@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_28</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>TC_29</t>
+  </si>
+  <si>
+    <t>Check the field accepts letter or not</t>
+  </si>
+  <si>
+    <t>Can not type
+letters</t>
+  </si>
+  <si>
+    <t>TC_30</t>
+  </si>
+  <si>
+    <t>Check the field acceepts anything other then numbers
+or not</t>
+  </si>
+  <si>
+    <t>TC_31</t>
+  </si>
+  <si>
+    <t>Check the field accepts invalid number or not</t>
+  </si>
+  <si>
+    <t>TC_32</t>
+  </si>
+  <si>
+    <t>Check the field has any limit or not</t>
+  </si>
+  <si>
+    <t>Should not be submitted and showed an error 
+massage of limitations</t>
+  </si>
+  <si>
+    <t>Can not submit. Length limitation is
+defined</t>
+  </si>
+  <si>
+    <t>TC_33</t>
+  </si>
+  <si>
+    <t>Check the field accepts more then 11 digit or not</t>
+  </si>
+  <si>
+    <t>TC_34</t>
+  </si>
+  <si>
+    <t>Check the field accepts less then 11 digit or not</t>
+  </si>
+  <si>
+    <t>TC_35</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>no data</t>
+  </si>
+  <si>
+    <t>TC_36</t>
+  </si>
+  <si>
+    <t>Check the field accepts valid password or not</t>
+  </si>
+  <si>
+    <t>TC_37</t>
+  </si>
+  <si>
+    <t>Check the field accepts 7 digits or not</t>
+  </si>
+  <si>
+    <t>TC_38</t>
+  </si>
+  <si>
+    <t>Check the field accepts 8 digits or not</t>
+  </si>
+  <si>
+    <t>TC_39</t>
+  </si>
+  <si>
+    <t>Check the field accepts 12 digits or not</t>
+  </si>
+  <si>
+    <t>TC_40</t>
+  </si>
+  <si>
+    <t>Have a defined length limitations to
+12 digits.</t>
+  </si>
+  <si>
+    <t>TC_41</t>
+  </si>
+  <si>
+    <t>TC_42</t>
+  </si>
+  <si>
+    <t>2010~!@#$*</t>
+  </si>
+  <si>
+    <t>But some special characters are
+not accepted like (,),%,",&amp; etc</t>
+  </si>
+  <si>
+    <t>TC_43</t>
+  </si>
+  <si>
+    <t>TC_44</t>
+  </si>
+  <si>
+    <t>12321!@#$</t>
+  </si>
+  <si>
+    <t>TC_45</t>
+  </si>
+  <si>
+    <t>asdf@#$hjk</t>
+  </si>
+  <si>
+    <t>TC_46</t>
+  </si>
+  <si>
+    <t>ASDFGHJKL</t>
+  </si>
+  <si>
+    <t>TC_47</t>
+  </si>
+  <si>
+    <t>asdfghjkl</t>
+  </si>
+  <si>
+    <t>TC_48</t>
+  </si>
+  <si>
+    <t>2010AnanHA@</t>
+  </si>
+  <si>
+    <t>TC_49</t>
+  </si>
+  <si>
+    <t>ফুয়াদ123456</t>
+  </si>
+  <si>
+    <t>TC_50</t>
+  </si>
+  <si>
+    <t>Retype Password</t>
+  </si>
+  <si>
+    <t>TC_51</t>
+  </si>
+  <si>
+    <t>Check the field accepts mismatched password or not</t>
+  </si>
+  <si>
+    <t>Password: 2010Anayh
+Retype: 2010Ananh</t>
+  </si>
+  <si>
+    <t>TC_52</t>
+  </si>
+  <si>
+    <t>TC_53</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -267,8 +479,13 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +514,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
         <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D2E9"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -331,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -358,6 +587,18 @@
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,7 +818,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="8.13"/>
     <col customWidth="1" min="2" max="2" width="23.63"/>
-    <col customWidth="1" min="3" max="3" width="36.88"/>
+    <col customWidth="1" min="3" max="3" width="40.13"/>
+    <col customWidth="1" min="4" max="4" width="18.25"/>
     <col customWidth="1" min="5" max="5" width="39.38"/>
     <col customWidth="1" min="6" max="6" width="26.88"/>
     <col customWidth="1" min="7" max="7" width="25.5"/>
@@ -829,6 +1071,15 @@
       <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="D14" s="7">
+        <v>12345.0</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
@@ -837,115 +1088,683 @@
       <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="D16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="D17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="D18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="D19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="D20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="D22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>47</v>
+        <v>69</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>67</v>
+        <v>78</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>69</v>
+        <v>81</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>71</v>
+        <v>84</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="4">
+        <v>6.5872465035E10</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1.6821320323232E13</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="4">
+        <v>8.801682132032E12</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1.68213203E8</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1.23456789E8</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="4">
+        <v>123456.0</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1234567.0</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1.23456789123E11</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1.23456789123E11</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1234567.0</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="B2:B12"/>
     <mergeCell ref="B13:B28"/>
+    <mergeCell ref="B29:B35"/>
+    <mergeCell ref="B36:B50"/>
+    <mergeCell ref="B51:B52"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>